<commit_message>
Correção de pequenos erros e usabilidade
</commit_message>
<xml_diff>
--- a/RelatorioContasCorrente.xlsx
+++ b/RelatorioContasCorrente.xlsx
@@ -137,7 +137,7 @@
         <v>3.25</v>
       </c>
       <c r="F2" t="n">
-        <v>45259.45933543982</v>
+        <v>45259.49596148148</v>
       </c>
       <c r="G2" t="n">
         <v>1.99999999575E9</v>
@@ -160,7 +160,7 @@
         <v>3.25</v>
       </c>
       <c r="F3" t="n">
-        <v>45259.45953748842</v>
+        <v>45259.49619430555</v>
       </c>
       <c r="G3" t="n">
         <v>1.9999999925E9</v>
@@ -183,7 +183,7 @@
         <v>3.25</v>
       </c>
       <c r="F4" t="n">
-        <v>45259.45956525463</v>
+        <v>45259.49622400463</v>
       </c>
       <c r="G4" t="n">
         <v>1.99999998925E9</v>
@@ -206,7 +206,7 @@
         <v>3.25</v>
       </c>
       <c r="F5" t="n">
-        <v>45259.45989680556</v>
+        <v>45259.49657850694</v>
       </c>
       <c r="G5" t="n">
         <v>1.999999986E9</v>
@@ -229,7 +229,7 @@
         <v>3.25</v>
       </c>
       <c r="F6" t="n">
-        <v>45259.46017215278</v>
+        <v>45259.4968712037</v>
       </c>
       <c r="G6" t="n">
         <v>1.99999998275E9</v>
@@ -252,7 +252,7 @@
         <v>3.25</v>
       </c>
       <c r="F7" t="n">
-        <v>45259.46022082176</v>
+        <v>45259.496924375</v>
       </c>
       <c r="G7" t="n">
         <v>1.9999999795E9</v>
@@ -275,7 +275,7 @@
         <v>3.25</v>
       </c>
       <c r="F8" t="n">
-        <v>45259.460522939815</v>
+        <v>45259.497244756945</v>
       </c>
       <c r="G8" t="n">
         <v>1.99999997625E9</v>
@@ -298,7 +298,7 @@
         <v>3.25</v>
       </c>
       <c r="F9" t="n">
-        <v>45259.46077172454</v>
+        <v>45259.49751269676</v>
       </c>
       <c r="G9" t="n">
         <v>1.999999973E9</v>
@@ -321,7 +321,7 @@
         <v>3.25</v>
       </c>
       <c r="F10" t="n">
-        <v>45259.460833703706</v>
+        <v>45259.497580972224</v>
       </c>
       <c r="G10" t="n">
         <v>1.99999996975E9</v>
@@ -344,7 +344,7 @@
         <v>3.25</v>
       </c>
       <c r="F11" t="n">
-        <v>45259.46110878472</v>
+        <v>45259.4978718287</v>
       </c>
       <c r="G11" t="n">
         <v>1.9999999665E9</v>
@@ -367,7 +367,7 @@
         <v>3.25</v>
       </c>
       <c r="F12" t="n">
-        <v>45259.461408159725</v>
+        <v>45259.49818141204</v>
       </c>
       <c r="G12" t="n">
         <v>1.99999996325E9</v>
@@ -390,7 +390,7 @@
         <v>3.25</v>
       </c>
       <c r="F13" t="n">
-        <v>45259.46150197917</v>
+        <v>45259.498268773146</v>
       </c>
       <c r="G13" t="n">
         <v>1.99999996E9</v>
@@ -413,7 +413,7 @@
         <v>3.25</v>
       </c>
       <c r="F14" t="n">
-        <v>45259.46180358796</v>
+        <v>45259.49860806713</v>
       </c>
       <c r="G14" t="n">
         <v>1.99999995675E9</v>
@@ -436,7 +436,7 @@
         <v>3.25</v>
       </c>
       <c r="F15" t="n">
-        <v>45259.46201790509</v>
+        <v>45259.49883331019</v>
       </c>
       <c r="G15" t="n">
         <v>1.9999999535E9</v>
@@ -459,7 +459,7 @@
         <v>3.25</v>
       </c>
       <c r="F16" t="n">
-        <v>45259.4621365162</v>
+        <v>45259.49896023148</v>
       </c>
       <c r="G16" t="n">
         <v>1.99999995025E9</v>
@@ -482,7 +482,7 @@
         <v>3.25</v>
       </c>
       <c r="F17" t="n">
-        <v>45259.46248008102</v>
+        <v>45259.49932715278</v>
       </c>
       <c r="G17" t="n">
         <v>1.999999947E9</v>
@@ -505,7 +505,7 @@
         <v>3.25</v>
       </c>
       <c r="F18" t="n">
-        <v>45259.462738622686</v>
+        <v>45259.49959344907</v>
       </c>
       <c r="G18" t="n">
         <v>1.99999994375E9</v>
@@ -528,7 +528,7 @@
         <v>3.25</v>
       </c>
       <c r="F19" t="n">
-        <v>45259.46285015046</v>
+        <v>45259.499716238424</v>
       </c>
       <c r="G19" t="n">
         <v>1.9999999405E9</v>
@@ -551,7 +551,7 @@
         <v>3.25</v>
       </c>
       <c r="F20" t="n">
-        <v>45259.46318461806</v>
+        <v>45259.500064872685</v>
       </c>
       <c r="G20" t="n">
         <v>1.99999993725E9</v>
@@ -574,7 +574,7 @@
         <v>3.25</v>
       </c>
       <c r="F21" t="n">
-        <v>45259.46338689815</v>
+        <v>45259.500276631945</v>
       </c>
       <c r="G21" t="n">
         <v>1.999999934E9</v>
@@ -597,7 +597,7 @@
         <v>3.25</v>
       </c>
       <c r="F22" t="n">
-        <v>45259.46352344907</v>
+        <v>45259.50042986111</v>
       </c>
       <c r="G22" t="n">
         <v>1.99999993075E9</v>
@@ -620,7 +620,7 @@
         <v>3.25</v>
       </c>
       <c r="F23" t="n">
-        <v>45259.463932743056</v>
+        <v>45259.50081430555</v>
       </c>
       <c r="G23" t="n">
         <v>1.9999999275E9</v>
@@ -643,7 +643,7 @@
         <v>3.25</v>
       </c>
       <c r="F24" t="n">
-        <v>45259.46414174769</v>
+        <v>45259.50101581019</v>
       </c>
       <c r="G24" t="n">
         <v>1.99999992425E9</v>
@@ -666,7 +666,7 @@
         <v>3.25</v>
       </c>
       <c r="F25" t="n">
-        <v>45259.46430099537</v>
+        <v>45259.50117337963</v>
       </c>
       <c r="G25" t="n">
         <v>1.999999921E9</v>
@@ -689,7 +689,7 @@
         <v>3.25</v>
       </c>
       <c r="F26" t="n">
-        <v>45259.46461594907</v>
+        <v>45259.5014859838</v>
       </c>
       <c r="G26" t="n">
         <v>1.99999991775E9</v>
@@ -712,7 +712,7 @@
         <v>3.25</v>
       </c>
       <c r="F27" t="n">
-        <v>45259.46470842593</v>
+        <v>45259.50158930555</v>
       </c>
       <c r="G27" t="n">
         <v>1.9999999145E9</v>
@@ -735,7 +735,7 @@
         <v>3.25</v>
       </c>
       <c r="F28" t="n">
-        <v>45259.46478236111</v>
+        <v>45259.501689398145</v>
       </c>
       <c r="G28" t="n">
         <v>1.99999991125E9</v>
@@ -758,7 +758,7 @@
         <v>3.25</v>
       </c>
       <c r="F29" t="n">
-        <v>45259.46490871528</v>
+        <v>45259.50185825231</v>
       </c>
       <c r="G29" t="n">
         <v>1.999999908E9</v>
@@ -781,7 +781,7 @@
         <v>3.25</v>
       </c>
       <c r="F30" t="n">
-        <v>45259.46497511574</v>
+        <v>45259.50193409722</v>
       </c>
       <c r="G30" t="n">
         <v>1.99999990475E9</v>
@@ -876,7 +876,7 @@
         <v>3.25</v>
       </c>
       <c r="F2" t="n">
-        <v>45259.45933546296</v>
+        <v>45259.49596148148</v>
       </c>
       <c r="G2" t="n">
         <v>33.25</v>
@@ -899,7 +899,7 @@
         <v>3.25</v>
       </c>
       <c r="F3" t="n">
-        <v>45259.45953748842</v>
+        <v>45259.49619430555</v>
       </c>
       <c r="G3" t="n">
         <v>36.5</v>
@@ -922,7 +922,7 @@
         <v>3.25</v>
       </c>
       <c r="F4" t="n">
-        <v>45259.45956525463</v>
+        <v>45259.49622400463</v>
       </c>
       <c r="G4" t="n">
         <v>39.75</v>
@@ -945,7 +945,7 @@
         <v>3.25</v>
       </c>
       <c r="F5" t="n">
-        <v>45259.45989680556</v>
+        <v>45259.49657850694</v>
       </c>
       <c r="G5" t="n">
         <v>43.0</v>
@@ -968,7 +968,7 @@
         <v>3.25</v>
       </c>
       <c r="F6" t="n">
-        <v>45259.46017215278</v>
+        <v>45259.4968712037</v>
       </c>
       <c r="G6" t="n">
         <v>46.25</v>
@@ -991,7 +991,7 @@
         <v>3.25</v>
       </c>
       <c r="F7" t="n">
-        <v>45259.46022082176</v>
+        <v>45259.496924375</v>
       </c>
       <c r="G7" t="n">
         <v>49.5</v>
@@ -1014,7 +1014,7 @@
         <v>3.25</v>
       </c>
       <c r="F8" t="n">
-        <v>45259.460522939815</v>
+        <v>45259.497244756945</v>
       </c>
       <c r="G8" t="n">
         <v>52.75</v>
@@ -1037,7 +1037,7 @@
         <v>3.25</v>
       </c>
       <c r="F9" t="n">
-        <v>45259.46077172454</v>
+        <v>45259.49751269676</v>
       </c>
       <c r="G9" t="n">
         <v>56.0</v>
@@ -1060,7 +1060,7 @@
         <v>3.25</v>
       </c>
       <c r="F10" t="n">
-        <v>45259.460833703706</v>
+        <v>45259.497580972224</v>
       </c>
       <c r="G10" t="n">
         <v>59.25</v>
@@ -1083,7 +1083,7 @@
         <v>3.25</v>
       </c>
       <c r="F11" t="n">
-        <v>45259.46110878472</v>
+        <v>45259.4978718287</v>
       </c>
       <c r="G11" t="n">
         <v>62.5</v>
@@ -1106,7 +1106,7 @@
         <v>3.25</v>
       </c>
       <c r="F12" t="n">
-        <v>45259.461408159725</v>
+        <v>45259.49818141204</v>
       </c>
       <c r="G12" t="n">
         <v>65.75</v>
@@ -1129,7 +1129,7 @@
         <v>3.25</v>
       </c>
       <c r="F13" t="n">
-        <v>45259.46150197917</v>
+        <v>45259.498268773146</v>
       </c>
       <c r="G13" t="n">
         <v>69.0</v>
@@ -1152,7 +1152,7 @@
         <v>3.25</v>
       </c>
       <c r="F14" t="n">
-        <v>45259.46180358796</v>
+        <v>45259.49860806713</v>
       </c>
       <c r="G14" t="n">
         <v>72.25</v>
@@ -1175,7 +1175,7 @@
         <v>3.25</v>
       </c>
       <c r="F15" t="n">
-        <v>45259.46201790509</v>
+        <v>45259.49883331019</v>
       </c>
       <c r="G15" t="n">
         <v>75.5</v>
@@ -1198,7 +1198,7 @@
         <v>3.25</v>
       </c>
       <c r="F16" t="n">
-        <v>45259.4621365162</v>
+        <v>45259.49896023148</v>
       </c>
       <c r="G16" t="n">
         <v>78.75</v>
@@ -1221,7 +1221,7 @@
         <v>3.25</v>
       </c>
       <c r="F17" t="n">
-        <v>45259.46248008102</v>
+        <v>45259.49932715278</v>
       </c>
       <c r="G17" t="n">
         <v>82.0</v>
@@ -1244,7 +1244,7 @@
         <v>3.25</v>
       </c>
       <c r="F18" t="n">
-        <v>45259.462738622686</v>
+        <v>45259.49959344907</v>
       </c>
       <c r="G18" t="n">
         <v>85.25</v>
@@ -1267,7 +1267,7 @@
         <v>3.25</v>
       </c>
       <c r="F19" t="n">
-        <v>45259.46285015046</v>
+        <v>45259.499716238424</v>
       </c>
       <c r="G19" t="n">
         <v>88.5</v>
@@ -1290,7 +1290,7 @@
         <v>3.25</v>
       </c>
       <c r="F20" t="n">
-        <v>45259.46318461806</v>
+        <v>45259.500064872685</v>
       </c>
       <c r="G20" t="n">
         <v>91.75</v>
@@ -1313,7 +1313,7 @@
         <v>3.25</v>
       </c>
       <c r="F21" t="n">
-        <v>45259.46338689815</v>
+        <v>45259.500276631945</v>
       </c>
       <c r="G21" t="n">
         <v>95.0</v>
@@ -1336,7 +1336,7 @@
         <v>3.25</v>
       </c>
       <c r="F22" t="n">
-        <v>45259.46352344907</v>
+        <v>45259.50042986111</v>
       </c>
       <c r="G22" t="n">
         <v>98.25</v>
@@ -1359,7 +1359,7 @@
         <v>3.25</v>
       </c>
       <c r="F23" t="n">
-        <v>45259.463932743056</v>
+        <v>45259.50081430555</v>
       </c>
       <c r="G23" t="n">
         <v>101.5</v>
@@ -1382,7 +1382,7 @@
         <v>3.25</v>
       </c>
       <c r="F24" t="n">
-        <v>45259.46414174769</v>
+        <v>45259.50101581019</v>
       </c>
       <c r="G24" t="n">
         <v>104.75</v>
@@ -1405,7 +1405,7 @@
         <v>3.25</v>
       </c>
       <c r="F25" t="n">
-        <v>45259.46430099537</v>
+        <v>45259.50117337963</v>
       </c>
       <c r="G25" t="n">
         <v>108.0</v>
@@ -1428,7 +1428,7 @@
         <v>3.25</v>
       </c>
       <c r="F26" t="n">
-        <v>45259.46461594907</v>
+        <v>45259.5014859838</v>
       </c>
       <c r="G26" t="n">
         <v>111.25</v>
@@ -1451,7 +1451,7 @@
         <v>3.25</v>
       </c>
       <c r="F27" t="n">
-        <v>45259.46470842593</v>
+        <v>45259.50158930555</v>
       </c>
       <c r="G27" t="n">
         <v>114.5</v>
@@ -1474,7 +1474,7 @@
         <v>3.25</v>
       </c>
       <c r="F28" t="n">
-        <v>45259.46478236111</v>
+        <v>45259.501689398145</v>
       </c>
       <c r="G28" t="n">
         <v>117.75</v>
@@ -1497,7 +1497,7 @@
         <v>3.25</v>
       </c>
       <c r="F29" t="n">
-        <v>45259.46490871528</v>
+        <v>45259.50185825231</v>
       </c>
       <c r="G29" t="n">
         <v>121.0</v>
@@ -1520,7 +1520,7 @@
         <v>3.25</v>
       </c>
       <c r="F30" t="n">
-        <v>45259.46497511574</v>
+        <v>45259.50193409722</v>
       </c>
       <c r="G30" t="n">
         <v>124.25</v>

</xml_diff>